<commit_message>
add classes in project
</commit_message>
<xml_diff>
--- a/Project/ProjectActivity.xlsx
+++ b/Project/ProjectActivity.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\CodeBank\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2CA50F-664F-426A-B5AE-5A4BF783A8EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35FBE21-1A2F-4A36-A59D-A6505FFF8D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{771DB91A-6DDE-4F61-8817-59B50CD031F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{771DB91A-6DDE-4F61-8817-59B50CD031F4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Activitys" sheetId="1" r:id="rId1"/>
+    <sheet name="Class" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="59">
   <si>
     <t>MainActivity</t>
   </si>
@@ -74,12 +75,6 @@
     <t>INVISTA EM CODECOIN</t>
   </si>
   <si>
-    <t>Cliente</t>
-  </si>
-  <si>
-    <t>Str Nome</t>
-  </si>
-  <si>
     <t>Str CPF</t>
   </si>
   <si>
@@ -89,18 +84,6 @@
     <t>Str Email</t>
   </si>
   <si>
-    <t>Str Endereço</t>
-  </si>
-  <si>
-    <t>Extrato Historico</t>
-  </si>
-  <si>
-    <t>Float SaldoAtual</t>
-  </si>
-  <si>
-    <t>CodeCard cartão</t>
-  </si>
-  <si>
     <t>Str Senha</t>
   </si>
   <si>
@@ -110,9 +93,6 @@
     <t>Doc</t>
   </si>
   <si>
-    <t>Investir</t>
-  </si>
-  <si>
     <t>Eai Pia!</t>
   </si>
   <si>
@@ -138,6 +118,102 @@
   </si>
   <si>
     <t>Termos e condições</t>
+  </si>
+  <si>
+    <t>ActivityLogin</t>
+  </si>
+  <si>
+    <t>ActivityRegister</t>
+  </si>
+  <si>
+    <t>ActivityMain</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Activity Class</t>
+  </si>
+  <si>
+    <t>Client client</t>
+  </si>
+  <si>
+    <t>FindCpf</t>
+  </si>
+  <si>
+    <t>VerifyClient</t>
+  </si>
+  <si>
+    <t>Str Name</t>
+  </si>
+  <si>
+    <t>Str PassWord</t>
+  </si>
+  <si>
+    <t>Str adress</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>VerifyPassWord</t>
+  </si>
+  <si>
+    <t>Extract historic</t>
+  </si>
+  <si>
+    <t>CodeCard card</t>
+  </si>
+  <si>
+    <t>Invest</t>
+  </si>
+  <si>
+    <t>PayTicket</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>ForgetPassword</t>
+  </si>
+  <si>
+    <t>Str cpf</t>
+  </si>
+  <si>
+    <t>CreateClient</t>
+  </si>
+  <si>
+    <t>ValidateDatas</t>
+  </si>
+  <si>
+    <t>VerifyCheckedTerms</t>
+  </si>
+  <si>
+    <t>ReadTerms</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>Balance</t>
+  </si>
+  <si>
+    <t>Float currentBalance</t>
+  </si>
+  <si>
+    <t>ViewBalanceButton</t>
+  </si>
+  <si>
+    <t>Balance balance</t>
+  </si>
+  <si>
+    <t>List historic</t>
+  </si>
+  <si>
+    <t>MovimentationBalance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Float valueMoney</t>
   </si>
 </sst>
 </file>
@@ -196,7 +272,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -281,6 +357,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="25">
     <border>
@@ -558,7 +640,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -603,6 +685,75 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -630,75 +781,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -718,6 +800,41 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1040,7 +1157,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1050,32 +1167,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFC992B9-F321-41FF-8B43-E43DDE45A3BE}">
   <dimension ref="B1:AK72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AG17" sqref="AG17"/>
+    <sheetView topLeftCell="A5" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:37" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:37" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="34"/>
-      <c r="M2" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
-      <c r="P2" s="37"/>
-      <c r="X2" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y2" s="38"/>
-      <c r="Z2" s="38"/>
-      <c r="AA2" s="39"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="71"/>
+      <c r="M2" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="60"/>
+      <c r="Q2" s="71"/>
+      <c r="X2" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y2" s="61"/>
+      <c r="Z2" s="61"/>
+      <c r="AA2" s="62"/>
+      <c r="AB2" s="71"/>
     </row>
     <row r="3" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
@@ -1126,15 +1246,15 @@
       <c r="I4" s="5"/>
       <c r="J4" s="18"/>
       <c r="M4" s="4"/>
-      <c r="N4" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="O4" s="40"/>
-      <c r="P4" s="40"/>
-      <c r="Q4" s="40"/>
-      <c r="R4" s="40"/>
-      <c r="S4" s="40"/>
-      <c r="T4" s="40"/>
+      <c r="N4" s="63" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" s="63"/>
+      <c r="P4" s="63"/>
+      <c r="Q4" s="63"/>
+      <c r="R4" s="63"/>
+      <c r="S4" s="63"/>
+      <c r="T4" s="63"/>
       <c r="U4" s="6"/>
       <c r="X4" s="4"/>
       <c r="Y4" s="5"/>
@@ -1160,23 +1280,23 @@
       <c r="I5" s="10"/>
       <c r="J5" s="18"/>
       <c r="M5" s="4"/>
-      <c r="N5" s="40"/>
-      <c r="O5" s="40"/>
-      <c r="P5" s="40"/>
-      <c r="Q5" s="40"/>
-      <c r="R5" s="40"/>
-      <c r="S5" s="40"/>
-      <c r="T5" s="40"/>
+      <c r="N5" s="63"/>
+      <c r="O5" s="63"/>
+      <c r="P5" s="63"/>
+      <c r="Q5" s="63"/>
+      <c r="R5" s="63"/>
+      <c r="S5" s="63"/>
+      <c r="T5" s="63"/>
       <c r="U5" s="6"/>
       <c r="X5" s="4"/>
       <c r="Y5" s="5"/>
-      <c r="Z5" s="48" t="s">
-        <v>31</v>
-      </c>
-      <c r="AA5" s="48"/>
-      <c r="AB5" s="48"/>
-      <c r="AC5" s="48"/>
-      <c r="AD5" s="48"/>
+      <c r="Z5" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA5" s="32"/>
+      <c r="AB5" s="32"/>
+      <c r="AC5" s="32"/>
+      <c r="AD5" s="32"/>
       <c r="AE5" s="5"/>
       <c r="AF5" s="6"/>
       <c r="AI5" s="27"/>
@@ -1194,23 +1314,23 @@
       <c r="I6" s="11"/>
       <c r="J6" s="20"/>
       <c r="M6" s="4"/>
-      <c r="N6" s="40"/>
-      <c r="O6" s="40"/>
-      <c r="P6" s="40"/>
-      <c r="Q6" s="40"/>
-      <c r="R6" s="40"/>
-      <c r="S6" s="40"/>
-      <c r="T6" s="40"/>
+      <c r="N6" s="63"/>
+      <c r="O6" s="63"/>
+      <c r="P6" s="63"/>
+      <c r="Q6" s="63"/>
+      <c r="R6" s="63"/>
+      <c r="S6" s="63"/>
+      <c r="T6" s="63"/>
       <c r="U6" s="6"/>
       <c r="X6" s="4"/>
       <c r="Y6" s="5"/>
-      <c r="Z6" s="48" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA6" s="48"/>
-      <c r="AB6" s="48"/>
-      <c r="AC6" s="48"/>
-      <c r="AD6" s="48"/>
+      <c r="Z6" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA6" s="32"/>
+      <c r="AB6" s="32"/>
+      <c r="AC6" s="32"/>
+      <c r="AD6" s="32"/>
       <c r="AE6" s="5"/>
       <c r="AF6" s="6"/>
       <c r="AI6" s="28"/>
@@ -1218,7 +1338,7 @@
       <c r="AK6" s="28"/>
     </row>
     <row r="7" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="34" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="66"/>
@@ -1248,13 +1368,13 @@
       <c r="U7" s="6"/>
       <c r="X7" s="4"/>
       <c r="Y7" s="5"/>
-      <c r="Z7" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA7" s="48"/>
-      <c r="AB7" s="48"/>
-      <c r="AC7" s="48"/>
-      <c r="AD7" s="48"/>
+      <c r="Z7" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA7" s="32"/>
+      <c r="AB7" s="32"/>
+      <c r="AC7" s="32"/>
+      <c r="AD7" s="32"/>
       <c r="AE7" s="5"/>
       <c r="AF7" s="6"/>
       <c r="AI7" s="24"/>
@@ -1262,7 +1382,7 @@
       <c r="AK7" s="24"/>
     </row>
     <row r="8" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="58"/>
+      <c r="B8" s="43"/>
       <c r="C8" s="68"/>
       <c r="D8" s="67"/>
       <c r="E8" s="68"/>
@@ -1282,13 +1402,13 @@
       <c r="U8" s="6"/>
       <c r="X8" s="4"/>
       <c r="Y8" s="5"/>
-      <c r="Z8" s="48" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA8" s="48"/>
-      <c r="AB8" s="48"/>
-      <c r="AC8" s="48"/>
-      <c r="AD8" s="48"/>
+      <c r="Z8" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA8" s="32"/>
+      <c r="AB8" s="32"/>
+      <c r="AC8" s="32"/>
+      <c r="AD8" s="32"/>
       <c r="AE8" s="5"/>
       <c r="AF8" s="6"/>
       <c r="AI8" s="29"/>
@@ -1296,26 +1416,26 @@
       <c r="AK8" s="29"/>
     </row>
     <row r="9" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="50"/>
-      <c r="I9" s="50"/>
-      <c r="J9" s="51"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="36"/>
       <c r="M9" s="4"/>
       <c r="N9" s="5"/>
-      <c r="O9" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="P9" s="41"/>
-      <c r="Q9" s="41"/>
-      <c r="R9" s="41"/>
-      <c r="S9" s="41"/>
+      <c r="O9" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="P9" s="33"/>
+      <c r="Q9" s="33"/>
+      <c r="R9" s="33"/>
+      <c r="S9" s="33"/>
       <c r="T9" s="5"/>
       <c r="U9" s="6"/>
       <c r="X9" s="4"/>
@@ -1332,24 +1452,24 @@
       <c r="AK9" s="30"/>
     </row>
     <row r="10" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="52"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="54"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="39"/>
       <c r="M10" s="4"/>
       <c r="N10" s="5"/>
-      <c r="O10" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="P10" s="41"/>
-      <c r="Q10" s="41"/>
-      <c r="R10" s="41"/>
-      <c r="S10" s="41"/>
+      <c r="O10" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="P10" s="33"/>
+      <c r="Q10" s="33"/>
+      <c r="R10" s="33"/>
+      <c r="S10" s="33"/>
       <c r="T10" s="5"/>
       <c r="U10" s="6"/>
       <c r="X10" s="4"/>
@@ -1366,15 +1486,15 @@
       <c r="AK10" s="31"/>
     </row>
     <row r="11" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="58"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="59"/>
-      <c r="H11" s="59"/>
-      <c r="I11" s="59"/>
-      <c r="J11" s="60"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="45"/>
       <c r="M11" s="4"/>
       <c r="N11" s="5"/>
       <c r="O11" s="21"/>
@@ -1386,35 +1506,35 @@
       <c r="U11" s="6"/>
       <c r="X11" s="4"/>
       <c r="Y11" s="5"/>
-      <c r="Z11" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA11" s="48"/>
-      <c r="AB11" s="48"/>
-      <c r="AC11" s="48"/>
-      <c r="AD11" s="48"/>
+      <c r="Z11" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA11" s="32"/>
+      <c r="AB11" s="32"/>
+      <c r="AC11" s="32"/>
+      <c r="AD11" s="32"/>
       <c r="AE11" s="5"/>
       <c r="AF11" s="6"/>
     </row>
     <row r="12" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="49" t="s">
+      <c r="B12" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="51"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="36"/>
       <c r="M12" s="4"/>
       <c r="N12" s="5"/>
-      <c r="P12" s="41" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q12" s="41"/>
-      <c r="R12" s="41"/>
+      <c r="P12" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q12" s="33"/>
+      <c r="R12" s="33"/>
       <c r="S12" s="21"/>
       <c r="T12" s="5"/>
       <c r="U12" s="6"/>
@@ -1429,15 +1549,15 @@
       <c r="AF12" s="6"/>
     </row>
     <row r="13" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="52"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="53"/>
-      <c r="I13" s="53"/>
-      <c r="J13" s="54"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="39"/>
       <c r="M13" s="4"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
@@ -1458,15 +1578,15 @@
       <c r="AF13" s="6"/>
     </row>
     <row r="14" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="58"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="59"/>
-      <c r="F14" s="59"/>
-      <c r="G14" s="59"/>
-      <c r="H14" s="59"/>
-      <c r="I14" s="59"/>
-      <c r="J14" s="60"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="45"/>
       <c r="M14" s="4"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
@@ -1487,17 +1607,17 @@
       <c r="AF14" s="6"/>
     </row>
     <row r="15" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="49" t="s">
+      <c r="B15" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="50"/>
-      <c r="I15" s="50"/>
-      <c r="J15" s="51"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="36"/>
       <c r="M15" s="4"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
@@ -1518,15 +1638,15 @@
       <c r="AF15" s="6"/>
     </row>
     <row r="16" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="52"/>
-      <c r="C16" s="53"/>
-      <c r="D16" s="53"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="53"/>
-      <c r="H16" s="53"/>
-      <c r="I16" s="53"/>
-      <c r="J16" s="54"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="39"/>
       <c r="M16" s="4"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
@@ -1547,15 +1667,15 @@
       <c r="AF16" s="6"/>
     </row>
     <row r="17" spans="2:32" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="52"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="53"/>
-      <c r="I17" s="53"/>
-      <c r="J17" s="54"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="39"/>
       <c r="M17" s="4"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
@@ -1576,15 +1696,15 @@
       <c r="AF17" s="6"/>
     </row>
     <row r="18" spans="2:32" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="55"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56"/>
-      <c r="H18" s="56"/>
-      <c r="I18" s="56"/>
-      <c r="J18" s="57"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="42"/>
       <c r="M18" s="7"/>
       <c r="N18" s="8"/>
       <c r="O18" s="8"/>
@@ -1606,89 +1726,16 @@
     </row>
     <row r="19" spans="2:32" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="2:32" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="2:32" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="2:32" ht="48" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B22" s="61" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="62"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="63"/>
-    </row>
-    <row r="23" spans="2:32" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="43"/>
-      <c r="D23" s="46" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23" s="47"/>
-    </row>
-    <row r="24" spans="2:32" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="43"/>
-      <c r="D24" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" s="47"/>
-    </row>
-    <row r="25" spans="2:32" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="43"/>
-      <c r="D25" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="E25" s="47"/>
-    </row>
-    <row r="26" spans="2:32" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="43"/>
-      <c r="D26" s="46" t="s">
-        <v>24</v>
-      </c>
-      <c r="E26" s="47"/>
-    </row>
-    <row r="27" spans="2:32" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="43"/>
-      <c r="D27" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="47"/>
-    </row>
-    <row r="28" spans="2:32" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" s="43"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="13"/>
-    </row>
-    <row r="29" spans="2:32" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29" s="43"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="13"/>
-    </row>
-    <row r="30" spans="2:32" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="C30" s="45"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="23"/>
-    </row>
+    <row r="21" spans="2:32" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:32" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:32" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:32" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:32" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="2:32" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:32" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:32" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:32" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:32" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="2:32" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="2:32" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1732,27 +1779,7 @@
     <row r="71" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="72" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="Z11:AD11"/>
-    <mergeCell ref="P12:R12"/>
-    <mergeCell ref="B15:J18"/>
-    <mergeCell ref="B12:J14"/>
-    <mergeCell ref="B9:J11"/>
-    <mergeCell ref="O10:S10"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
+  <mergeCells count="22">
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="M2:P2"/>
     <mergeCell ref="X2:AA2"/>
@@ -1769,6 +1796,469 @@
     <mergeCell ref="Z6:AD6"/>
     <mergeCell ref="Z5:AD5"/>
     <mergeCell ref="J7:J8"/>
+    <mergeCell ref="Z11:AD11"/>
+    <mergeCell ref="P12:R12"/>
+    <mergeCell ref="B15:J18"/>
+    <mergeCell ref="B12:J14"/>
+    <mergeCell ref="B9:J11"/>
+    <mergeCell ref="O10:S10"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BDCAEAD-7C4D-47DD-A11B-8969E7EDE7E7}">
+  <dimension ref="B1:J32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:10" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="81" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="83"/>
+      <c r="G2" s="81" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="85"/>
+    </row>
+    <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B4" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="54"/>
+      <c r="G4" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="54"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="47"/>
+      <c r="D5" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="51"/>
+      <c r="G5" s="46" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="72"/>
+      <c r="I5" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" s="51"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="47"/>
+      <c r="D6" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="51"/>
+      <c r="G6" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="72"/>
+      <c r="I6" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" s="51"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="47"/>
+      <c r="D7" s="50" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="51"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="72"/>
+      <c r="I7" s="50" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7" s="51"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="47"/>
+      <c r="D8" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="51"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="72"/>
+      <c r="I8" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="51"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="46" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="47"/>
+      <c r="D9" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="51"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="72"/>
+      <c r="I9" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="J9" s="51"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="47"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="51"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="72"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="13"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="47"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="51"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="72"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="13"/>
+    </row>
+    <row r="12" spans="2:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="49"/>
+      <c r="D12" s="73"/>
+      <c r="E12" s="74"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="23"/>
+    </row>
+    <row r="13" spans="2:10" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B14" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="53"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="54"/>
+      <c r="G14" s="52" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="53"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="54"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="47"/>
+      <c r="D15" s="50" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="51"/>
+      <c r="G15" s="46" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="72"/>
+      <c r="I15" s="75" t="s">
+        <v>47</v>
+      </c>
+      <c r="J15" s="51"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="47"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="51"/>
+      <c r="G16" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="H16" s="72"/>
+      <c r="I16" s="75" t="s">
+        <v>48</v>
+      </c>
+      <c r="J16" s="51"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="46"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="51"/>
+      <c r="G17" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="72"/>
+      <c r="I17" s="75" t="s">
+        <v>49</v>
+      </c>
+      <c r="J17" s="51"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="46"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="51"/>
+      <c r="G18" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="72"/>
+      <c r="I18" s="75" t="s">
+        <v>50</v>
+      </c>
+      <c r="J18" s="51"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="46"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="51"/>
+      <c r="G19" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="72"/>
+      <c r="I19" s="75"/>
+      <c r="J19" s="51"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="46"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="13"/>
+      <c r="G20" s="77"/>
+      <c r="H20" s="78"/>
+      <c r="I20" s="76"/>
+      <c r="J20" s="13"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="46"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="13"/>
+      <c r="G21" s="77"/>
+      <c r="H21" s="78"/>
+      <c r="I21" s="76"/>
+      <c r="J21" s="13"/>
+    </row>
+    <row r="22" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="48"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="23"/>
+      <c r="G22" s="79"/>
+      <c r="H22" s="80"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="23"/>
+    </row>
+    <row r="23" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="G24" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="H24" s="53"/>
+      <c r="I24" s="53"/>
+      <c r="J24" s="54"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G25" s="46" t="s">
+        <v>32</v>
+      </c>
+      <c r="H25" s="47"/>
+      <c r="I25" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="J25" s="51"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G26" s="46" t="s">
+        <v>55</v>
+      </c>
+      <c r="H26" s="47"/>
+      <c r="I26" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="J26" s="51"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G27" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="H27" s="47"/>
+      <c r="I27" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="J27" s="51"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G28" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="H28" s="47"/>
+      <c r="I28" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="J28" s="51"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G29" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="H29" s="47"/>
+      <c r="I29" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="J29" s="51"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G30" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="H30" s="47"/>
+      <c r="I30" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="J30" s="51"/>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G31" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="H31" s="47"/>
+      <c r="I31" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="J31" s="51"/>
+    </row>
+    <row r="32" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G32" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="H32" s="49"/>
+      <c r="I32" s="73" t="s">
+        <v>51</v>
+      </c>
+      <c r="J32" s="74"/>
+    </row>
+  </sheetData>
+  <mergeCells count="75">
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="G24:J24"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
translated ids of loginActivity
</commit_message>
<xml_diff>
--- a/Project/ProjectActivity.xlsx
+++ b/Project/ProjectActivity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\CodeBank\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35FBE21-1A2F-4A36-A59D-A6505FFF8D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8568D0C2-26D7-461B-88BB-770667B8540C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{771DB91A-6DDE-4F61-8817-59B50CD031F4}"/>
   </bookViews>
@@ -84,9 +84,6 @@
     <t>Str Email</t>
   </si>
   <si>
-    <t>Str Senha</t>
-  </si>
-  <si>
     <t>Ted</t>
   </si>
   <si>
@@ -214,6 +211,9 @@
   </si>
   <si>
     <t xml:space="preserve">  Float valueMoney</t>
+  </si>
+  <si>
+    <t>Str passWord</t>
   </si>
 </sst>
 </file>
@@ -640,7 +640,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -685,156 +685,147 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1175,27 +1166,27 @@
   <sheetData>
     <row r="1" spans="2:37" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:37" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="71"/>
-      <c r="M2" s="58" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" s="59"/>
-      <c r="O2" s="59"/>
-      <c r="P2" s="60"/>
-      <c r="Q2" s="71"/>
-      <c r="X2" s="58" t="s">
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="32"/>
+      <c r="M2" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="Y2" s="61"/>
-      <c r="Z2" s="61"/>
-      <c r="AA2" s="62"/>
-      <c r="AB2" s="71"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="32"/>
+      <c r="X2" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y2" s="43"/>
+      <c r="Z2" s="43"/>
+      <c r="AA2" s="44"/>
+      <c r="AB2" s="32"/>
     </row>
     <row r="3" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
@@ -1233,28 +1224,28 @@
     </row>
     <row r="4" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="17"/>
-      <c r="C4" s="64" t="s">
+      <c r="C4" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="64" t="s">
+      <c r="G4" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="64"/>
+      <c r="H4" s="47"/>
       <c r="I4" s="5"/>
       <c r="J4" s="18"/>
       <c r="M4" s="4"/>
-      <c r="N4" s="63" t="s">
-        <v>18</v>
-      </c>
-      <c r="O4" s="63"/>
-      <c r="P4" s="63"/>
-      <c r="Q4" s="63"/>
-      <c r="R4" s="63"/>
-      <c r="S4" s="63"/>
-      <c r="T4" s="63"/>
+      <c r="N4" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" s="45"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="45"/>
+      <c r="R4" s="45"/>
+      <c r="S4" s="45"/>
+      <c r="T4" s="45"/>
       <c r="U4" s="6"/>
       <c r="X4" s="4"/>
       <c r="Y4" s="5"/>
@@ -1280,23 +1271,23 @@
       <c r="I5" s="10"/>
       <c r="J5" s="18"/>
       <c r="M5" s="4"/>
-      <c r="N5" s="63"/>
-      <c r="O5" s="63"/>
-      <c r="P5" s="63"/>
-      <c r="Q5" s="63"/>
-      <c r="R5" s="63"/>
-      <c r="S5" s="63"/>
-      <c r="T5" s="63"/>
+      <c r="N5" s="45"/>
+      <c r="O5" s="45"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="45"/>
+      <c r="R5" s="45"/>
+      <c r="S5" s="45"/>
+      <c r="T5" s="45"/>
       <c r="U5" s="6"/>
       <c r="X5" s="4"/>
       <c r="Y5" s="5"/>
-      <c r="Z5" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA5" s="32"/>
-      <c r="AB5" s="32"/>
-      <c r="AC5" s="32"/>
-      <c r="AD5" s="32"/>
+      <c r="Z5" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA5" s="54"/>
+      <c r="AB5" s="54"/>
+      <c r="AC5" s="54"/>
+      <c r="AD5" s="54"/>
       <c r="AE5" s="5"/>
       <c r="AF5" s="6"/>
       <c r="AI5" s="27"/>
@@ -1314,23 +1305,23 @@
       <c r="I6" s="11"/>
       <c r="J6" s="20"/>
       <c r="M6" s="4"/>
-      <c r="N6" s="63"/>
-      <c r="O6" s="63"/>
-      <c r="P6" s="63"/>
-      <c r="Q6" s="63"/>
-      <c r="R6" s="63"/>
-      <c r="S6" s="63"/>
-      <c r="T6" s="63"/>
+      <c r="N6" s="45"/>
+      <c r="O6" s="45"/>
+      <c r="P6" s="45"/>
+      <c r="Q6" s="45"/>
+      <c r="R6" s="45"/>
+      <c r="S6" s="45"/>
+      <c r="T6" s="45"/>
       <c r="U6" s="6"/>
       <c r="X6" s="4"/>
       <c r="Y6" s="5"/>
-      <c r="Z6" s="32" t="s">
+      <c r="Z6" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="AA6" s="32"/>
-      <c r="AB6" s="32"/>
-      <c r="AC6" s="32"/>
-      <c r="AD6" s="32"/>
+      <c r="AA6" s="54"/>
+      <c r="AB6" s="54"/>
+      <c r="AC6" s="54"/>
+      <c r="AD6" s="54"/>
       <c r="AE6" s="5"/>
       <c r="AF6" s="6"/>
       <c r="AI6" s="28"/>
@@ -1338,23 +1329,23 @@
       <c r="AK6" s="28"/>
     </row>
     <row r="7" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="66"/>
-      <c r="D7" s="65" t="s">
+      <c r="C7" s="49"/>
+      <c r="D7" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="66"/>
-      <c r="F7" s="65" t="s">
+      <c r="E7" s="49"/>
+      <c r="F7" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="66"/>
-      <c r="H7" s="65" t="s">
+      <c r="G7" s="49"/>
+      <c r="H7" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="66"/>
-      <c r="J7" s="69" t="s">
+      <c r="I7" s="49"/>
+      <c r="J7" s="55" t="s">
         <v>8</v>
       </c>
       <c r="M7" s="4"/>
@@ -1368,13 +1359,13 @@
       <c r="U7" s="6"/>
       <c r="X7" s="4"/>
       <c r="Y7" s="5"/>
-      <c r="Z7" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA7" s="32"/>
-      <c r="AB7" s="32"/>
-      <c r="AC7" s="32"/>
-      <c r="AD7" s="32"/>
+      <c r="Z7" s="54" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA7" s="54"/>
+      <c r="AB7" s="54"/>
+      <c r="AC7" s="54"/>
+      <c r="AD7" s="54"/>
       <c r="AE7" s="5"/>
       <c r="AF7" s="6"/>
       <c r="AI7" s="24"/>
@@ -1382,15 +1373,15 @@
       <c r="AK7" s="24"/>
     </row>
     <row r="8" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="43"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="68"/>
-      <c r="H8" s="67"/>
-      <c r="I8" s="68"/>
-      <c r="J8" s="70"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="56"/>
       <c r="M8" s="4"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
@@ -1402,13 +1393,13 @@
       <c r="U8" s="6"/>
       <c r="X8" s="4"/>
       <c r="Y8" s="5"/>
-      <c r="Z8" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA8" s="32"/>
-      <c r="AB8" s="32"/>
-      <c r="AC8" s="32"/>
-      <c r="AD8" s="32"/>
+      <c r="Z8" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA8" s="54"/>
+      <c r="AB8" s="54"/>
+      <c r="AC8" s="54"/>
+      <c r="AD8" s="54"/>
       <c r="AE8" s="5"/>
       <c r="AF8" s="6"/>
       <c r="AI8" s="29"/>
@@ -1416,26 +1407,26 @@
       <c r="AK8" s="29"/>
     </row>
     <row r="9" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="36"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="58"/>
       <c r="M9" s="4"/>
       <c r="N9" s="5"/>
-      <c r="O9" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="P9" s="33"/>
-      <c r="Q9" s="33"/>
-      <c r="R9" s="33"/>
-      <c r="S9" s="33"/>
+      <c r="O9" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="P9" s="46"/>
+      <c r="Q9" s="46"/>
+      <c r="R9" s="46"/>
+      <c r="S9" s="46"/>
       <c r="T9" s="5"/>
       <c r="U9" s="6"/>
       <c r="X9" s="4"/>
@@ -1452,24 +1443,24 @@
       <c r="AK9" s="30"/>
     </row>
     <row r="10" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="37"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="39"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="60"/>
+      <c r="I10" s="60"/>
+      <c r="J10" s="61"/>
       <c r="M10" s="4"/>
       <c r="N10" s="5"/>
-      <c r="O10" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="P10" s="33"/>
-      <c r="Q10" s="33"/>
-      <c r="R10" s="33"/>
-      <c r="S10" s="33"/>
+      <c r="O10" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="P10" s="46"/>
+      <c r="Q10" s="46"/>
+      <c r="R10" s="46"/>
+      <c r="S10" s="46"/>
       <c r="T10" s="5"/>
       <c r="U10" s="6"/>
       <c r="X10" s="4"/>
@@ -1486,15 +1477,15 @@
       <c r="AK10" s="31"/>
     </row>
     <row r="11" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="43"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="45"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="65"/>
+      <c r="I11" s="65"/>
+      <c r="J11" s="66"/>
       <c r="M11" s="4"/>
       <c r="N11" s="5"/>
       <c r="O11" s="21"/>
@@ -1506,35 +1497,35 @@
       <c r="U11" s="6"/>
       <c r="X11" s="4"/>
       <c r="Y11" s="5"/>
-      <c r="Z11" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA11" s="32"/>
-      <c r="AB11" s="32"/>
-      <c r="AC11" s="32"/>
-      <c r="AD11" s="32"/>
+      <c r="Z11" s="54" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA11" s="54"/>
+      <c r="AB11" s="54"/>
+      <c r="AC11" s="54"/>
+      <c r="AD11" s="54"/>
       <c r="AE11" s="5"/>
       <c r="AF11" s="6"/>
     </row>
     <row r="12" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="36"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="57"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="58"/>
       <c r="M12" s="4"/>
       <c r="N12" s="5"/>
-      <c r="P12" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q12" s="33"/>
-      <c r="R12" s="33"/>
+      <c r="P12" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q12" s="46"/>
+      <c r="R12" s="46"/>
       <c r="S12" s="21"/>
       <c r="T12" s="5"/>
       <c r="U12" s="6"/>
@@ -1549,15 +1540,15 @@
       <c r="AF12" s="6"/>
     </row>
     <row r="13" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="37"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="39"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="60"/>
+      <c r="I13" s="60"/>
+      <c r="J13" s="61"/>
       <c r="M13" s="4"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
@@ -1578,15 +1569,15 @@
       <c r="AF13" s="6"/>
     </row>
     <row r="14" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="43"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
-      <c r="J14" s="45"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="65"/>
+      <c r="J14" s="66"/>
       <c r="M14" s="4"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
@@ -1607,17 +1598,17 @@
       <c r="AF14" s="6"/>
     </row>
     <row r="15" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="36"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="57"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="58"/>
       <c r="M15" s="4"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
@@ -1638,15 +1629,15 @@
       <c r="AF15" s="6"/>
     </row>
     <row r="16" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="37"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="39"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="60"/>
+      <c r="J16" s="61"/>
       <c r="M16" s="4"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
@@ -1667,15 +1658,15 @@
       <c r="AF16" s="6"/>
     </row>
     <row r="17" spans="2:32" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="37"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="39"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="60"/>
+      <c r="J17" s="61"/>
       <c r="M17" s="4"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
@@ -1696,15 +1687,15 @@
       <c r="AF17" s="6"/>
     </row>
     <row r="18" spans="2:32" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="40"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="42"/>
+      <c r="B18" s="62"/>
+      <c r="C18" s="63"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="63"/>
+      <c r="F18" s="63"/>
+      <c r="G18" s="63"/>
+      <c r="H18" s="63"/>
+      <c r="I18" s="63"/>
+      <c r="J18" s="64"/>
       <c r="M18" s="7"/>
       <c r="N18" s="8"/>
       <c r="O18" s="8"/>
@@ -1780,6 +1771,12 @@
     <row r="72" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="Z11:AD11"/>
+    <mergeCell ref="P12:R12"/>
+    <mergeCell ref="B15:J18"/>
+    <mergeCell ref="B12:J14"/>
+    <mergeCell ref="B9:J11"/>
+    <mergeCell ref="O10:S10"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="M2:P2"/>
     <mergeCell ref="X2:AA2"/>
@@ -1796,12 +1793,6 @@
     <mergeCell ref="Z6:AD6"/>
     <mergeCell ref="Z5:AD5"/>
     <mergeCell ref="J7:J8"/>
-    <mergeCell ref="Z11:AD11"/>
-    <mergeCell ref="P12:R12"/>
-    <mergeCell ref="B15:J18"/>
-    <mergeCell ref="B12:J14"/>
-    <mergeCell ref="B9:J11"/>
-    <mergeCell ref="O10:S10"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1813,7 +1804,7 @@
   <dimension ref="B1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="L12" sqref="L12:L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1826,393 +1817,392 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="75" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="82"/>
+      <c r="G2" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="83"/>
-      <c r="G2" s="81" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="85"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="77"/>
     </row>
     <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="78" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="80"/>
+      <c r="G4" s="78" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="80"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="71" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="72"/>
+      <c r="D5" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="70"/>
+      <c r="G5" s="71" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="72"/>
+      <c r="I5" s="69" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="70"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="71" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="72"/>
+      <c r="D6" s="69" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="70"/>
+      <c r="G6" s="71" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="72"/>
+      <c r="I6" s="69" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="70"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="72"/>
+      <c r="D7" s="69" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="70"/>
+      <c r="G7" s="71"/>
+      <c r="H7" s="72"/>
+      <c r="I7" s="69" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" s="70"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="71" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="72"/>
+      <c r="D8" s="69" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="70"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="72"/>
+      <c r="I8" s="69" t="s">
+        <v>37</v>
+      </c>
+      <c r="J8" s="70"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="72"/>
+      <c r="D9" s="69" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="70"/>
+      <c r="G9" s="71"/>
+      <c r="H9" s="72"/>
+      <c r="I9" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="54"/>
-      <c r="G4" s="52" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="54"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="50" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="51"/>
-      <c r="G5" s="46" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="72"/>
-      <c r="I5" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" s="51"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="46" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="47"/>
-      <c r="D6" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="51"/>
-      <c r="G6" s="46" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" s="72"/>
-      <c r="I6" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" s="51"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="50" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="51"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="50" t="s">
+      <c r="J9" s="70"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="J7" s="51"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="47"/>
-      <c r="D8" s="50" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="51"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="J8" s="51"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="46" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="50" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="51"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="J9" s="51"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="51"/>
-      <c r="G10" s="46"/>
+      <c r="C10" s="72"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="70"/>
+      <c r="G10" s="71"/>
       <c r="H10" s="72"/>
       <c r="I10" s="12"/>
       <c r="J10" s="13"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="46" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="47"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="51"/>
-      <c r="G11" s="46"/>
+      <c r="B11" s="71" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="72"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="70"/>
+      <c r="G11" s="71"/>
       <c r="H11" s="72"/>
       <c r="I11" s="12"/>
       <c r="J11" s="13"/>
     </row>
     <row r="12" spans="2:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="48" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="73"/>
-      <c r="E12" s="74"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="49"/>
+      <c r="B12" s="73" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="74"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="68"/>
+      <c r="G12" s="73"/>
+      <c r="H12" s="74"/>
       <c r="I12" s="22"/>
       <c r="J12" s="23"/>
     </row>
     <row r="13" spans="2:10" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B14" s="52" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="53"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="54"/>
-      <c r="G14" s="52" t="s">
-        <v>28</v>
-      </c>
-      <c r="H14" s="53"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="54"/>
+      <c r="B14" s="78" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="79"/>
+      <c r="D14" s="79"/>
+      <c r="E14" s="80"/>
+      <c r="G14" s="78" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" s="79"/>
+      <c r="I14" s="79"/>
+      <c r="J14" s="80"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="71" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="72"/>
+      <c r="D15" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="70"/>
+      <c r="G15" s="71" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" s="72"/>
+      <c r="I15" s="69" t="s">
+        <v>46</v>
+      </c>
+      <c r="J15" s="70"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="72"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="70"/>
+      <c r="G16" s="71" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" s="72"/>
+      <c r="I16" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="J16" s="70"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="71"/>
+      <c r="C17" s="72"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="70"/>
+      <c r="G17" s="71" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="72"/>
+      <c r="I17" s="69" t="s">
+        <v>48</v>
+      </c>
+      <c r="J17" s="70"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="71"/>
+      <c r="C18" s="72"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="70"/>
+      <c r="G18" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="72"/>
+      <c r="I18" s="69" t="s">
+        <v>49</v>
+      </c>
+      <c r="J18" s="70"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="71"/>
+      <c r="C19" s="72"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="70"/>
+      <c r="G19" s="71" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="47"/>
-      <c r="D15" s="50" t="s">
-        <v>57</v>
-      </c>
-      <c r="E15" s="51"/>
-      <c r="G15" s="46" t="s">
-        <v>32</v>
-      </c>
-      <c r="H15" s="72"/>
-      <c r="I15" s="75" t="s">
-        <v>47</v>
-      </c>
-      <c r="J15" s="51"/>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="46" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" s="47"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="51"/>
-      <c r="G16" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="H16" s="72"/>
-      <c r="I16" s="75" t="s">
-        <v>48</v>
-      </c>
-      <c r="J16" s="51"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="46"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="51"/>
-      <c r="G17" s="46" t="s">
-        <v>12</v>
-      </c>
-      <c r="H17" s="72"/>
-      <c r="I17" s="75" t="s">
-        <v>49</v>
-      </c>
-      <c r="J17" s="51"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="46"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="51"/>
-      <c r="G18" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="72"/>
-      <c r="I18" s="75" t="s">
-        <v>50</v>
-      </c>
-      <c r="J18" s="51"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="46"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="51"/>
-      <c r="G19" s="46" t="s">
-        <v>15</v>
-      </c>
       <c r="H19" s="72"/>
-      <c r="I19" s="75"/>
-      <c r="J19" s="51"/>
+      <c r="I19" s="69"/>
+      <c r="J19" s="70"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="46"/>
-      <c r="C20" s="47"/>
+      <c r="B20" s="71"/>
+      <c r="C20" s="72"/>
       <c r="D20" s="12"/>
       <c r="E20" s="13"/>
-      <c r="G20" s="77"/>
-      <c r="H20" s="78"/>
-      <c r="I20" s="76"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="12"/>
       <c r="J20" s="13"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="46"/>
-      <c r="C21" s="47"/>
+      <c r="B21" s="71"/>
+      <c r="C21" s="72"/>
       <c r="D21" s="12"/>
       <c r="E21" s="13"/>
-      <c r="G21" s="77"/>
-      <c r="H21" s="78"/>
-      <c r="I21" s="76"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="12"/>
       <c r="J21" s="13"/>
     </row>
     <row r="22" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="48"/>
-      <c r="C22" s="49"/>
+      <c r="B22" s="73"/>
+      <c r="C22" s="74"/>
       <c r="D22" s="22"/>
       <c r="E22" s="23"/>
-      <c r="G22" s="79"/>
-      <c r="H22" s="80"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="36"/>
       <c r="I22" s="22"/>
       <c r="J22" s="23"/>
     </row>
     <row r="23" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="G24" s="52" t="s">
-        <v>29</v>
-      </c>
-      <c r="H24" s="53"/>
-      <c r="I24" s="53"/>
-      <c r="J24" s="54"/>
+      <c r="G24" s="78" t="s">
+        <v>28</v>
+      </c>
+      <c r="H24" s="79"/>
+      <c r="I24" s="79"/>
+      <c r="J24" s="80"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G25" s="46" t="s">
-        <v>32</v>
-      </c>
-      <c r="H25" s="47"/>
-      <c r="I25" s="50" t="s">
+      <c r="G25" s="71" t="s">
+        <v>31</v>
+      </c>
+      <c r="H25" s="72"/>
+      <c r="I25" s="69" t="s">
+        <v>53</v>
+      </c>
+      <c r="J25" s="70"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G26" s="71" t="s">
         <v>54</v>
       </c>
-      <c r="J25" s="51"/>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G26" s="46" t="s">
-        <v>55</v>
-      </c>
-      <c r="H26" s="47"/>
-      <c r="I26" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="J26" s="51"/>
+      <c r="H26" s="72"/>
+      <c r="I26" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="J26" s="70"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G27" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="H27" s="47"/>
-      <c r="I27" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="J27" s="51"/>
+      <c r="G27" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="H27" s="72"/>
+      <c r="I27" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="J27" s="70"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G28" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="H28" s="47"/>
-      <c r="I28" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="J28" s="51"/>
+      <c r="G28" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="H28" s="72"/>
+      <c r="I28" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="J28" s="70"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G29" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="H29" s="47"/>
-      <c r="I29" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="J29" s="51"/>
+      <c r="G29" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="H29" s="72"/>
+      <c r="I29" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="J29" s="70"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G30" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="H30" s="47"/>
-      <c r="I30" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="J30" s="51"/>
+      <c r="G30" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="H30" s="72"/>
+      <c r="I30" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="J30" s="70"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G31" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="H31" s="47"/>
-      <c r="I31" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="J31" s="51"/>
+      <c r="G31" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="H31" s="72"/>
+      <c r="I31" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="J31" s="70"/>
     </row>
     <row r="32" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G32" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H32" s="49"/>
-      <c r="I32" s="73" t="s">
-        <v>51</v>
-      </c>
-      <c r="J32" s="74"/>
+      <c r="G32" s="73" t="s">
+        <v>50</v>
+      </c>
+      <c r="H32" s="74"/>
+      <c r="I32" s="67" t="s">
+        <v>50</v>
+      </c>
+      <c r="J32" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="G28:H28"/>
     <mergeCell ref="I28:J28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="I31:J31"/>
     <mergeCell ref="G25:H25"/>
     <mergeCell ref="I25:J25"/>
     <mergeCell ref="G26:H26"/>
@@ -2221,12 +2211,16 @@
     <mergeCell ref="I27:J27"/>
     <mergeCell ref="I19:J19"/>
     <mergeCell ref="G24:J24"/>
-    <mergeCell ref="I16:J16"/>
     <mergeCell ref="I17:J17"/>
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="I18:J18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="I16:J16"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="G11:H11"/>
@@ -2236,29 +2230,26 @@
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G17:H17"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add balance and client class
</commit_message>
<xml_diff>
--- a/Project/ProjectActivity.xlsx
+++ b/Project/ProjectActivity.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\CodeBank\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\OneDrive\workspace\git\CodeBank\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35FBE21-1A2F-4A36-A59D-A6505FFF8D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E79C663-32F5-466D-94AD-A776B073373E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{771DB91A-6DDE-4F61-8817-59B50CD031F4}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{771DB91A-6DDE-4F61-8817-59B50CD031F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Activitys" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
   <si>
     <t>MainActivity</t>
   </si>
@@ -81,12 +81,6 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Str Email</t>
-  </si>
-  <si>
-    <t>Str Senha</t>
-  </si>
-  <si>
     <t>Ted</t>
   </si>
   <si>
@@ -141,15 +135,6 @@
     <t>FindCpf</t>
   </si>
   <si>
-    <t>VerifyClient</t>
-  </si>
-  <si>
-    <t>Str Name</t>
-  </si>
-  <si>
-    <t>Str PassWord</t>
-  </si>
-  <si>
     <t>Str adress</t>
   </si>
   <si>
@@ -214,6 +199,15 @@
   </si>
   <si>
     <t xml:space="preserve">  Float valueMoney</t>
+  </si>
+  <si>
+    <t>Str password</t>
+  </si>
+  <si>
+    <t>Str name</t>
+  </si>
+  <si>
+    <t>Str email</t>
   </si>
 </sst>
 </file>
@@ -640,7 +634,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -685,156 +679,147 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1167,7 +1152,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFC992B9-F321-41FF-8B43-E43DDE45A3BE}">
   <dimension ref="B1:AK72"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="B22" sqref="B22:E30"/>
     </sheetView>
   </sheetViews>
@@ -1175,27 +1160,27 @@
   <sheetData>
     <row r="1" spans="2:37" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:37" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="71"/>
-      <c r="M2" s="58" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" s="59"/>
-      <c r="O2" s="59"/>
-      <c r="P2" s="60"/>
-      <c r="Q2" s="71"/>
-      <c r="X2" s="58" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y2" s="61"/>
-      <c r="Z2" s="61"/>
-      <c r="AA2" s="62"/>
-      <c r="AB2" s="71"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="32"/>
+      <c r="M2" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="32"/>
+      <c r="X2" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y2" s="43"/>
+      <c r="Z2" s="43"/>
+      <c r="AA2" s="44"/>
+      <c r="AB2" s="32"/>
     </row>
     <row r="3" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
@@ -1233,28 +1218,28 @@
     </row>
     <row r="4" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="17"/>
-      <c r="C4" s="64" t="s">
+      <c r="C4" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="64" t="s">
+      <c r="G4" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="64"/>
+      <c r="H4" s="47"/>
       <c r="I4" s="5"/>
       <c r="J4" s="18"/>
       <c r="M4" s="4"/>
-      <c r="N4" s="63" t="s">
-        <v>18</v>
-      </c>
-      <c r="O4" s="63"/>
-      <c r="P4" s="63"/>
-      <c r="Q4" s="63"/>
-      <c r="R4" s="63"/>
-      <c r="S4" s="63"/>
-      <c r="T4" s="63"/>
+      <c r="N4" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4" s="45"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="45"/>
+      <c r="R4" s="45"/>
+      <c r="S4" s="45"/>
+      <c r="T4" s="45"/>
       <c r="U4" s="6"/>
       <c r="X4" s="4"/>
       <c r="Y4" s="5"/>
@@ -1280,23 +1265,23 @@
       <c r="I5" s="10"/>
       <c r="J5" s="18"/>
       <c r="M5" s="4"/>
-      <c r="N5" s="63"/>
-      <c r="O5" s="63"/>
-      <c r="P5" s="63"/>
-      <c r="Q5" s="63"/>
-      <c r="R5" s="63"/>
-      <c r="S5" s="63"/>
-      <c r="T5" s="63"/>
+      <c r="N5" s="45"/>
+      <c r="O5" s="45"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="45"/>
+      <c r="R5" s="45"/>
+      <c r="S5" s="45"/>
+      <c r="T5" s="45"/>
       <c r="U5" s="6"/>
       <c r="X5" s="4"/>
       <c r="Y5" s="5"/>
-      <c r="Z5" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA5" s="32"/>
-      <c r="AB5" s="32"/>
-      <c r="AC5" s="32"/>
-      <c r="AD5" s="32"/>
+      <c r="Z5" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA5" s="54"/>
+      <c r="AB5" s="54"/>
+      <c r="AC5" s="54"/>
+      <c r="AD5" s="54"/>
       <c r="AE5" s="5"/>
       <c r="AF5" s="6"/>
       <c r="AI5" s="27"/>
@@ -1314,23 +1299,23 @@
       <c r="I6" s="11"/>
       <c r="J6" s="20"/>
       <c r="M6" s="4"/>
-      <c r="N6" s="63"/>
-      <c r="O6" s="63"/>
-      <c r="P6" s="63"/>
-      <c r="Q6" s="63"/>
-      <c r="R6" s="63"/>
-      <c r="S6" s="63"/>
-      <c r="T6" s="63"/>
+      <c r="N6" s="45"/>
+      <c r="O6" s="45"/>
+      <c r="P6" s="45"/>
+      <c r="Q6" s="45"/>
+      <c r="R6" s="45"/>
+      <c r="S6" s="45"/>
+      <c r="T6" s="45"/>
       <c r="U6" s="6"/>
       <c r="X6" s="4"/>
       <c r="Y6" s="5"/>
-      <c r="Z6" s="32" t="s">
+      <c r="Z6" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="AA6" s="32"/>
-      <c r="AB6" s="32"/>
-      <c r="AC6" s="32"/>
-      <c r="AD6" s="32"/>
+      <c r="AA6" s="54"/>
+      <c r="AB6" s="54"/>
+      <c r="AC6" s="54"/>
+      <c r="AD6" s="54"/>
       <c r="AE6" s="5"/>
       <c r="AF6" s="6"/>
       <c r="AI6" s="28"/>
@@ -1338,23 +1323,23 @@
       <c r="AK6" s="28"/>
     </row>
     <row r="7" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="66"/>
-      <c r="D7" s="65" t="s">
+      <c r="C7" s="49"/>
+      <c r="D7" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="66"/>
-      <c r="F7" s="65" t="s">
+      <c r="E7" s="49"/>
+      <c r="F7" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="66"/>
-      <c r="H7" s="65" t="s">
+      <c r="G7" s="49"/>
+      <c r="H7" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="66"/>
-      <c r="J7" s="69" t="s">
+      <c r="I7" s="49"/>
+      <c r="J7" s="55" t="s">
         <v>8</v>
       </c>
       <c r="M7" s="4"/>
@@ -1368,13 +1353,13 @@
       <c r="U7" s="6"/>
       <c r="X7" s="4"/>
       <c r="Y7" s="5"/>
-      <c r="Z7" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA7" s="32"/>
-      <c r="AB7" s="32"/>
-      <c r="AC7" s="32"/>
-      <c r="AD7" s="32"/>
+      <c r="Z7" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA7" s="54"/>
+      <c r="AB7" s="54"/>
+      <c r="AC7" s="54"/>
+      <c r="AD7" s="54"/>
       <c r="AE7" s="5"/>
       <c r="AF7" s="6"/>
       <c r="AI7" s="24"/>
@@ -1382,15 +1367,15 @@
       <c r="AK7" s="24"/>
     </row>
     <row r="8" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="43"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="68"/>
-      <c r="H8" s="67"/>
-      <c r="I8" s="68"/>
-      <c r="J8" s="70"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="56"/>
       <c r="M8" s="4"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
@@ -1402,13 +1387,13 @@
       <c r="U8" s="6"/>
       <c r="X8" s="4"/>
       <c r="Y8" s="5"/>
-      <c r="Z8" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA8" s="32"/>
-      <c r="AB8" s="32"/>
-      <c r="AC8" s="32"/>
-      <c r="AD8" s="32"/>
+      <c r="Z8" s="54" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA8" s="54"/>
+      <c r="AB8" s="54"/>
+      <c r="AC8" s="54"/>
+      <c r="AD8" s="54"/>
       <c r="AE8" s="5"/>
       <c r="AF8" s="6"/>
       <c r="AI8" s="29"/>
@@ -1416,26 +1401,26 @@
       <c r="AK8" s="29"/>
     </row>
     <row r="9" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="36"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="58"/>
       <c r="M9" s="4"/>
       <c r="N9" s="5"/>
-      <c r="O9" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="P9" s="33"/>
-      <c r="Q9" s="33"/>
-      <c r="R9" s="33"/>
-      <c r="S9" s="33"/>
+      <c r="O9" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="P9" s="46"/>
+      <c r="Q9" s="46"/>
+      <c r="R9" s="46"/>
+      <c r="S9" s="46"/>
       <c r="T9" s="5"/>
       <c r="U9" s="6"/>
       <c r="X9" s="4"/>
@@ -1452,24 +1437,24 @@
       <c r="AK9" s="30"/>
     </row>
     <row r="10" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="37"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="39"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="60"/>
+      <c r="I10" s="60"/>
+      <c r="J10" s="61"/>
       <c r="M10" s="4"/>
       <c r="N10" s="5"/>
-      <c r="O10" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="P10" s="33"/>
-      <c r="Q10" s="33"/>
-      <c r="R10" s="33"/>
-      <c r="S10" s="33"/>
+      <c r="O10" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="P10" s="46"/>
+      <c r="Q10" s="46"/>
+      <c r="R10" s="46"/>
+      <c r="S10" s="46"/>
       <c r="T10" s="5"/>
       <c r="U10" s="6"/>
       <c r="X10" s="4"/>
@@ -1486,15 +1471,15 @@
       <c r="AK10" s="31"/>
     </row>
     <row r="11" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="43"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="45"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="65"/>
+      <c r="I11" s="65"/>
+      <c r="J11" s="66"/>
       <c r="M11" s="4"/>
       <c r="N11" s="5"/>
       <c r="O11" s="21"/>
@@ -1506,35 +1491,35 @@
       <c r="U11" s="6"/>
       <c r="X11" s="4"/>
       <c r="Y11" s="5"/>
-      <c r="Z11" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA11" s="32"/>
-      <c r="AB11" s="32"/>
-      <c r="AC11" s="32"/>
-      <c r="AD11" s="32"/>
+      <c r="Z11" s="54" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA11" s="54"/>
+      <c r="AB11" s="54"/>
+      <c r="AC11" s="54"/>
+      <c r="AD11" s="54"/>
       <c r="AE11" s="5"/>
       <c r="AF11" s="6"/>
     </row>
     <row r="12" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="36"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="57"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="58"/>
       <c r="M12" s="4"/>
       <c r="N12" s="5"/>
-      <c r="P12" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q12" s="33"/>
-      <c r="R12" s="33"/>
+      <c r="P12" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q12" s="46"/>
+      <c r="R12" s="46"/>
       <c r="S12" s="21"/>
       <c r="T12" s="5"/>
       <c r="U12" s="6"/>
@@ -1549,15 +1534,15 @@
       <c r="AF12" s="6"/>
     </row>
     <row r="13" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="37"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="39"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="60"/>
+      <c r="I13" s="60"/>
+      <c r="J13" s="61"/>
       <c r="M13" s="4"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
@@ -1578,15 +1563,15 @@
       <c r="AF13" s="6"/>
     </row>
     <row r="14" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="43"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
-      <c r="J14" s="45"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="65"/>
+      <c r="J14" s="66"/>
       <c r="M14" s="4"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
@@ -1607,17 +1592,17 @@
       <c r="AF14" s="6"/>
     </row>
     <row r="15" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="36"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="57"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="58"/>
       <c r="M15" s="4"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
@@ -1638,15 +1623,15 @@
       <c r="AF15" s="6"/>
     </row>
     <row r="16" spans="2:37" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="37"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="39"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="60"/>
+      <c r="J16" s="61"/>
       <c r="M16" s="4"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
@@ -1667,15 +1652,15 @@
       <c r="AF16" s="6"/>
     </row>
     <row r="17" spans="2:32" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="37"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="39"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="60"/>
+      <c r="J17" s="61"/>
       <c r="M17" s="4"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
@@ -1696,15 +1681,15 @@
       <c r="AF17" s="6"/>
     </row>
     <row r="18" spans="2:32" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="40"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="42"/>
+      <c r="B18" s="62"/>
+      <c r="C18" s="63"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="63"/>
+      <c r="F18" s="63"/>
+      <c r="G18" s="63"/>
+      <c r="H18" s="63"/>
+      <c r="I18" s="63"/>
+      <c r="J18" s="64"/>
       <c r="M18" s="7"/>
       <c r="N18" s="8"/>
       <c r="O18" s="8"/>
@@ -1780,6 +1765,12 @@
     <row r="72" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="Z11:AD11"/>
+    <mergeCell ref="P12:R12"/>
+    <mergeCell ref="B15:J18"/>
+    <mergeCell ref="B12:J14"/>
+    <mergeCell ref="B9:J11"/>
+    <mergeCell ref="O10:S10"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="M2:P2"/>
     <mergeCell ref="X2:AA2"/>
@@ -1796,12 +1787,6 @@
     <mergeCell ref="Z6:AD6"/>
     <mergeCell ref="Z5:AD5"/>
     <mergeCell ref="J7:J8"/>
-    <mergeCell ref="Z11:AD11"/>
-    <mergeCell ref="P12:R12"/>
-    <mergeCell ref="B15:J18"/>
-    <mergeCell ref="B12:J14"/>
-    <mergeCell ref="B9:J11"/>
-    <mergeCell ref="O10:S10"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1813,7 +1798,7 @@
   <dimension ref="B1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="B6" sqref="B6:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1826,393 +1811,392 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="81" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="83"/>
-      <c r="G2" s="81" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="85"/>
+      <c r="B2" s="75" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="82"/>
+      <c r="G2" s="75" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="77"/>
     </row>
     <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B4" s="52" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="54"/>
-      <c r="G4" s="52" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="54"/>
+      <c r="B4" s="78" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="80"/>
+      <c r="G4" s="78" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="80"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="72"/>
+      <c r="D5" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="70"/>
+      <c r="G5" s="71" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="72"/>
+      <c r="I5" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="70"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="71" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="72"/>
+      <c r="D6" s="69" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="70"/>
+      <c r="G6" s="71" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="72"/>
+      <c r="I6" s="69" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" s="70"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="71" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="72"/>
+      <c r="D7" s="69" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="70"/>
+      <c r="G7" s="71" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="72"/>
+      <c r="I7" s="69" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="70"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="71" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="72"/>
+      <c r="D8" s="69" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="70"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="72"/>
+      <c r="I8" s="69" t="s">
+        <v>40</v>
+      </c>
+      <c r="J8" s="70"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="71" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="72"/>
+      <c r="D9" s="69" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="70"/>
+      <c r="G9" s="71"/>
+      <c r="H9" s="72"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="70"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="71" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="50" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="51"/>
-      <c r="G5" s="46" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="72"/>
-      <c r="I5" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" s="51"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="46" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="47"/>
-      <c r="D6" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="51"/>
-      <c r="G6" s="46" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" s="72"/>
-      <c r="I6" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" s="51"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="50" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="51"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="50" t="s">
-        <v>39</v>
-      </c>
-      <c r="J7" s="51"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="47"/>
-      <c r="D8" s="50" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="51"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="J8" s="51"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="46" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="50" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="51"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="J9" s="51"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="51"/>
-      <c r="G10" s="46"/>
+      <c r="C10" s="72"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="70"/>
+      <c r="G10" s="71"/>
       <c r="H10" s="72"/>
       <c r="I10" s="12"/>
       <c r="J10" s="13"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="46" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="47"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="51"/>
-      <c r="G11" s="46"/>
+      <c r="B11" s="71" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="72"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="70"/>
+      <c r="G11" s="71"/>
       <c r="H11" s="72"/>
       <c r="I11" s="12"/>
       <c r="J11" s="13"/>
     </row>
     <row r="12" spans="2:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="48" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="73"/>
-      <c r="E12" s="74"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="49"/>
+      <c r="B12" s="73" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="74"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="68"/>
+      <c r="G12" s="73"/>
+      <c r="H12" s="74"/>
       <c r="I12" s="22"/>
       <c r="J12" s="23"/>
     </row>
     <row r="13" spans="2:10" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B14" s="52" t="s">
+      <c r="B14" s="78" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="79"/>
+      <c r="D14" s="79"/>
+      <c r="E14" s="80"/>
+      <c r="G14" s="78" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="79"/>
+      <c r="I14" s="79"/>
+      <c r="J14" s="80"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="71" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="72"/>
+      <c r="D15" s="69" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="53"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="54"/>
-      <c r="G14" s="52" t="s">
-        <v>28</v>
-      </c>
-      <c r="H14" s="53"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="54"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="47"/>
-      <c r="D15" s="50" t="s">
-        <v>57</v>
-      </c>
-      <c r="E15" s="51"/>
-      <c r="G15" s="46" t="s">
-        <v>32</v>
+      <c r="E15" s="70"/>
+      <c r="G15" s="71" t="s">
+        <v>30</v>
       </c>
       <c r="H15" s="72"/>
-      <c r="I15" s="75" t="s">
-        <v>47</v>
-      </c>
-      <c r="J15" s="51"/>
+      <c r="I15" s="69" t="s">
+        <v>42</v>
+      </c>
+      <c r="J15" s="70"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="46" t="s">
+      <c r="B16" s="71" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="72"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="70"/>
+      <c r="G16" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="72"/>
+      <c r="I16" s="69" t="s">
+        <v>43</v>
+      </c>
+      <c r="J16" s="70"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="71"/>
+      <c r="C17" s="72"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="70"/>
+      <c r="G17" s="71" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="72"/>
+      <c r="I17" s="69" t="s">
+        <v>44</v>
+      </c>
+      <c r="J17" s="70"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="71"/>
+      <c r="C18" s="72"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="70"/>
+      <c r="G18" s="71" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="47"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="51"/>
-      <c r="G16" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="H16" s="72"/>
-      <c r="I16" s="75" t="s">
-        <v>48</v>
-      </c>
-      <c r="J16" s="51"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="46"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="51"/>
-      <c r="G17" s="46" t="s">
-        <v>12</v>
-      </c>
-      <c r="H17" s="72"/>
-      <c r="I17" s="75" t="s">
-        <v>49</v>
-      </c>
-      <c r="J17" s="51"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="46"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="51"/>
-      <c r="G18" s="46" t="s">
-        <v>14</v>
-      </c>
       <c r="H18" s="72"/>
-      <c r="I18" s="75" t="s">
-        <v>50</v>
-      </c>
-      <c r="J18" s="51"/>
+      <c r="I18" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="J18" s="70"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="46"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="51"/>
-      <c r="G19" s="46" t="s">
-        <v>15</v>
+      <c r="B19" s="71"/>
+      <c r="C19" s="72"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="70"/>
+      <c r="G19" s="71" t="s">
+        <v>54</v>
       </c>
       <c r="H19" s="72"/>
-      <c r="I19" s="75"/>
-      <c r="J19" s="51"/>
+      <c r="I19" s="69"/>
+      <c r="J19" s="70"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="46"/>
-      <c r="C20" s="47"/>
+      <c r="B20" s="71"/>
+      <c r="C20" s="72"/>
       <c r="D20" s="12"/>
       <c r="E20" s="13"/>
-      <c r="G20" s="77"/>
-      <c r="H20" s="78"/>
-      <c r="I20" s="76"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="12"/>
       <c r="J20" s="13"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="46"/>
-      <c r="C21" s="47"/>
+      <c r="B21" s="71"/>
+      <c r="C21" s="72"/>
       <c r="D21" s="12"/>
       <c r="E21" s="13"/>
-      <c r="G21" s="77"/>
-      <c r="H21" s="78"/>
-      <c r="I21" s="76"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="12"/>
       <c r="J21" s="13"/>
     </row>
     <row r="22" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="48"/>
-      <c r="C22" s="49"/>
+      <c r="B22" s="73"/>
+      <c r="C22" s="74"/>
       <c r="D22" s="22"/>
       <c r="E22" s="23"/>
-      <c r="G22" s="79"/>
-      <c r="H22" s="80"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="36"/>
       <c r="I22" s="22"/>
       <c r="J22" s="23"/>
     </row>
     <row r="23" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="2:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="G24" s="52" t="s">
-        <v>29</v>
-      </c>
-      <c r="H24" s="53"/>
-      <c r="I24" s="53"/>
-      <c r="J24" s="54"/>
+      <c r="G24" s="78" t="s">
+        <v>27</v>
+      </c>
+      <c r="H24" s="79"/>
+      <c r="I24" s="79"/>
+      <c r="J24" s="80"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G25" s="46" t="s">
-        <v>32</v>
-      </c>
-      <c r="H25" s="47"/>
-      <c r="I25" s="50" t="s">
-        <v>54</v>
-      </c>
-      <c r="J25" s="51"/>
+      <c r="G25" s="71" t="s">
+        <v>30</v>
+      </c>
+      <c r="H25" s="72"/>
+      <c r="I25" s="69" t="s">
+        <v>49</v>
+      </c>
+      <c r="J25" s="70"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G26" s="46" t="s">
-        <v>55</v>
-      </c>
-      <c r="H26" s="47"/>
-      <c r="I26" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="J26" s="51"/>
+      <c r="G26" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="H26" s="72"/>
+      <c r="I26" s="69" t="s">
+        <v>46</v>
+      </c>
+      <c r="J26" s="70"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G27" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="H27" s="47"/>
-      <c r="I27" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="J27" s="51"/>
+      <c r="G27" s="71" t="s">
+        <v>46</v>
+      </c>
+      <c r="H27" s="72"/>
+      <c r="I27" s="69" t="s">
+        <v>46</v>
+      </c>
+      <c r="J27" s="70"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G28" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="H28" s="47"/>
-      <c r="I28" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="J28" s="51"/>
+      <c r="G28" s="71" t="s">
+        <v>46</v>
+      </c>
+      <c r="H28" s="72"/>
+      <c r="I28" s="69" t="s">
+        <v>46</v>
+      </c>
+      <c r="J28" s="70"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G29" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="H29" s="47"/>
-      <c r="I29" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="J29" s="51"/>
+      <c r="G29" s="71" t="s">
+        <v>46</v>
+      </c>
+      <c r="H29" s="72"/>
+      <c r="I29" s="69" t="s">
+        <v>46</v>
+      </c>
+      <c r="J29" s="70"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G30" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="H30" s="47"/>
-      <c r="I30" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="J30" s="51"/>
+      <c r="G30" s="71" t="s">
+        <v>46</v>
+      </c>
+      <c r="H30" s="72"/>
+      <c r="I30" s="69" t="s">
+        <v>46</v>
+      </c>
+      <c r="J30" s="70"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G31" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="H31" s="47"/>
-      <c r="I31" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="J31" s="51"/>
+      <c r="G31" s="71" t="s">
+        <v>46</v>
+      </c>
+      <c r="H31" s="72"/>
+      <c r="I31" s="69" t="s">
+        <v>46</v>
+      </c>
+      <c r="J31" s="70"/>
     </row>
     <row r="32" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G32" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="H32" s="49"/>
-      <c r="I32" s="73" t="s">
-        <v>51</v>
-      </c>
-      <c r="J32" s="74"/>
+      <c r="G32" s="73" t="s">
+        <v>46</v>
+      </c>
+      <c r="H32" s="74"/>
+      <c r="I32" s="67" t="s">
+        <v>46</v>
+      </c>
+      <c r="J32" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="G28:H28"/>
     <mergeCell ref="I28:J28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="I31:J31"/>
     <mergeCell ref="G25:H25"/>
     <mergeCell ref="I25:J25"/>
     <mergeCell ref="G26:H26"/>
@@ -2221,12 +2205,16 @@
     <mergeCell ref="I27:J27"/>
     <mergeCell ref="I19:J19"/>
     <mergeCell ref="G24:J24"/>
-    <mergeCell ref="I16:J16"/>
     <mergeCell ref="I17:J17"/>
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="I18:J18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="I16:J16"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="G11:H11"/>
@@ -2236,29 +2224,26 @@
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G17:H17"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>